<commit_message>
Updated main, reshuffled model, and excel document
</commit_message>
<xml_diff>
--- a/CS 598 Model Performance Records.xlsx
+++ b/CS 598 Model Performance Records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dHCP\Data\Neurodevelopmental-Phenotype-Prediction-Repro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53C68AF1-6057-48DC-B325-68899B764906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33E8046-C2E9-4D84-9B95-A4D3DC654B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CA969083-A445-499C-A790-35B849542B34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{CA969083-A445-499C-A790-35B849542B34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
   <si>
     <t>Model Run Name</t>
   </si>
@@ -174,6 +196,39 @@
   </si>
   <si>
     <t>Time (minutes)</t>
+  </si>
+  <si>
+    <t>Scan Age</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Reproduced / Original</t>
+  </si>
+  <si>
+    <t>Impatience Parameter (200)</t>
+  </si>
+  <si>
+    <t>Impatient Reshuffle (200)</t>
+  </si>
+  <si>
+    <t>Birth Age</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Sex Age</t>
+  </si>
+  <si>
+    <t>Impatience Parameter (200), Birth Age Indices</t>
+  </si>
+  <si>
+    <t>Impatience Parameter (200), Reshuffled Indices</t>
   </si>
 </sst>
 </file>
@@ -197,7 +252,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -205,14 +260,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AA7DBD-3193-4134-9CB6-B78985326199}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,9 +713,17 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="63.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +749,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -592,7 +769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -613,7 +790,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -629,8 +806,23 @@
       <c r="F4">
         <v>32.020000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="P4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="6"/>
+      <c r="T4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -649,14 +841,75 @@
       <c r="G5" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G6">
         <f>AVERAGE(E12:E98)</f>
         <v>444</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.72109999999999996</v>
+      </c>
+      <c r="N6" s="7">
+        <f>AVERAGE(M6:M9)</f>
+        <v>0.71627500000000011</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="2" cm="1">
+        <f t="array" ref="Q6:Q9">D7:D10</f>
+        <v>1.3348</v>
+      </c>
+      <c r="R6" s="7">
+        <f>AVERAGE(Q6:Q9)</f>
+        <v>1.2799500000000001</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U6" s="2" cm="1">
+        <f t="array" ref="U6:U9">D12:D15</f>
+        <v>0.30854999999999999</v>
+      </c>
+      <c r="V6" s="8">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(U6))</f>
+        <v>0.3443351375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -672,8 +925,29 @@
       <c r="F7">
         <v>31.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="P7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1.2455000000000001</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="T7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.37354964000000002</v>
+      </c>
+      <c r="V7" s="8"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -689,8 +963,29 @@
       <c r="F8">
         <v>31.92</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.70569999999999999</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="P8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1.2675000000000001</v>
+      </c>
+      <c r="R8" s="9"/>
+      <c r="T8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.36210096000000003</v>
+      </c>
+      <c r="V8" s="8"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -706,8 +1001,29 @@
       <c r="F9">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.75929999999999997</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="P9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1.272</v>
+      </c>
+      <c r="R9" s="10"/>
+      <c r="T9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0.33313995000000002</v>
+      </c>
+      <c r="V9" s="8"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -723,8 +1039,52 @@
       <c r="F10">
         <v>31.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" s="2" cm="1">
+        <f t="array" ref="M11:M14">D17:D20</f>
+        <v>0.68482505999999999</v>
+      </c>
+      <c r="N11" s="7">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(M11))</f>
+        <v>0.70360192750000006</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="2" cm="1">
+        <f t="array" ref="Q11:Q14">D22:D25</f>
+        <v>1.2532748</v>
+      </c>
+      <c r="R11" s="7">
+        <f>AVERAGE(Q11:Q14)</f>
+        <v>1.2647612750000001</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U11" s="2" cm="1">
+        <f t="array" ref="U11:U14">D37:D40</f>
+        <v>0.436888473</v>
+      </c>
+      <c r="V11" s="8">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(U11))</f>
+        <v>0.44045138824999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -743,8 +1103,29 @@
       <c r="F12">
         <v>10.62</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.67977995000000002</v>
+      </c>
+      <c r="N12" s="9"/>
+      <c r="P12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1.2592574000000001</v>
+      </c>
+      <c r="R12" s="9"/>
+      <c r="T12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0.45155960000000001</v>
+      </c>
+      <c r="V12" s="8"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -763,8 +1144,29 @@
       <c r="F13">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.72517010000000004</v>
+      </c>
+      <c r="N13" s="9"/>
+      <c r="P13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1.2651281000000001</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="T13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0.43527349999999998</v>
+      </c>
+      <c r="V13" s="8"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -783,8 +1185,29 @@
       <c r="F14">
         <v>9.94</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.72463259999999996</v>
+      </c>
+      <c r="N14" s="10"/>
+      <c r="P14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1.2813848000000001</v>
+      </c>
+      <c r="R14" s="10"/>
+      <c r="T14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0.43808397999999998</v>
+      </c>
+      <c r="V14" s="8"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -803,8 +1226,38 @@
       <c r="F15">
         <v>9.18</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" s="2" cm="1">
+        <f t="array" ref="M16:M19">D27:D30</f>
+        <v>0.54765039999999998</v>
+      </c>
+      <c r="N16" s="7">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(M16))</f>
+        <v>0.55791794250000004</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q16" s="2" cm="1">
+        <f t="array" ref="Q16:Q19">D32:D35</f>
+        <v>1.7301135000000001</v>
+      </c>
+      <c r="R16" s="7">
+        <f>AVERAGE(Q16:Q19)</f>
+        <v>1.7676751500000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -823,8 +1276,22 @@
       <c r="F17">
         <v>16.28</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.55219739999999995</v>
+      </c>
+      <c r="N17" s="9"/>
+      <c r="P17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1.7792435</v>
+      </c>
+      <c r="R17" s="9"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -843,8 +1310,22 @@
       <c r="F18">
         <v>9.94</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.56655776999999996</v>
+      </c>
+      <c r="N18" s="9"/>
+      <c r="P18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1.7104816</v>
+      </c>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -863,8 +1344,22 @@
       <c r="F19">
         <v>10.27</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.56526620000000005</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="P19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>1.850862</v>
+      </c>
+      <c r="R19" s="10"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -884,7 +1379,7 @@
         <v>11.48</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -904,7 +1399,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -924,7 +1419,7 @@
         <v>10.19</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -944,7 +1439,7 @@
         <v>8.64</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -964,7 +1459,7 @@
         <v>8.0299999999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -987,7 +1482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1010,7 +1505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1033,7 +1528,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1056,7 +1551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1242,5 +1737,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>